<commit_message>
Added leading zeros to NSC Themes, added Sustainable Farming Fund to appropriations
</commit_message>
<xml_diff>
--- a/xlsx/national-science-challenge-theme.xlsx
+++ b/xlsx/national-science-challenge-theme.xlsx
@@ -23,7 +23,7 @@
     <t xml:space="preserve">Definition</t>
   </si>
   <si>
-    <t xml:space="preserve">0101</t>
+    <t xml:space="preserve">00101</t>
   </si>
   <si>
     <t xml:space="preserve">Obesity</t>
@@ -32,31 +32,31 @@
     <t xml:space="preserve">NSC: A Better Start</t>
   </si>
   <si>
-    <t xml:space="preserve">0102</t>
+    <t xml:space="preserve">00102</t>
   </si>
   <si>
     <t xml:space="preserve">Literacy</t>
   </si>
   <si>
-    <t xml:space="preserve">0103</t>
+    <t xml:space="preserve">00103</t>
   </si>
   <si>
     <t xml:space="preserve">Big Data</t>
   </si>
   <si>
-    <t xml:space="preserve">0104</t>
+    <t xml:space="preserve">00104</t>
   </si>
   <si>
     <t xml:space="preserve">Youth Mental Health</t>
   </si>
   <si>
-    <t xml:space="preserve">0105</t>
+    <t xml:space="preserve">00105</t>
   </si>
   <si>
     <t xml:space="preserve">Māori Research</t>
   </si>
   <si>
-    <t xml:space="preserve">0201</t>
+    <t xml:space="preserve">00201</t>
   </si>
   <si>
     <t xml:space="preserve">Enabling independence and autonomy</t>
@@ -65,31 +65,31 @@
     <t xml:space="preserve">NSC: Ageing Well</t>
   </si>
   <si>
-    <t xml:space="preserve">0202</t>
+    <t xml:space="preserve">00202</t>
   </si>
   <si>
     <t xml:space="preserve">Ensuring a meaningful life through social integration and engagement</t>
   </si>
   <si>
-    <t xml:space="preserve">0203</t>
+    <t xml:space="preserve">00203</t>
   </si>
   <si>
     <t xml:space="preserve">Recognising at a societal level the value of ongoing contributions of knowledge and experience of older people</t>
   </si>
   <si>
-    <t xml:space="preserve">0204</t>
+    <t xml:space="preserve">00204</t>
   </si>
   <si>
     <t xml:space="preserve">Reducing disability</t>
   </si>
   <si>
-    <t xml:space="preserve">0205</t>
+    <t xml:space="preserve">00205</t>
   </si>
   <si>
     <t xml:space="preserve">Developing age-friendly environments</t>
   </si>
   <si>
-    <t xml:space="preserve">0301</t>
+    <t xml:space="preserve">00301</t>
   </si>
   <si>
     <t xml:space="preserve">Transforming Homes, Towns and Cities</t>
@@ -98,37 +98,37 @@
     <t xml:space="preserve">NSC: Building Better Homes, Towns and Cities</t>
   </si>
   <si>
-    <t xml:space="preserve">0302</t>
+    <t xml:space="preserve">00302</t>
   </si>
   <si>
     <t xml:space="preserve">Next Generation Information for Better Outcomes</t>
   </si>
   <si>
-    <t xml:space="preserve">0303</t>
+    <t xml:space="preserve">00303</t>
   </si>
   <si>
     <t xml:space="preserve">Supporting Success in Regional Settlements</t>
   </si>
   <si>
-    <t xml:space="preserve">0304</t>
+    <t xml:space="preserve">00304</t>
   </si>
   <si>
     <t xml:space="preserve">Shaping Places Future Neighbourhoods</t>
   </si>
   <si>
-    <t xml:space="preserve">0305</t>
+    <t xml:space="preserve">00305</t>
   </si>
   <si>
     <t xml:space="preserve">Evolving to Enhance Mauri</t>
   </si>
   <si>
-    <t xml:space="preserve">0306</t>
+    <t xml:space="preserve">00306</t>
   </si>
   <si>
     <t xml:space="preserve">Transforming the Building Industry</t>
   </si>
   <si>
-    <t xml:space="preserve">0401</t>
+    <t xml:space="preserve">00401</t>
   </si>
   <si>
     <t xml:space="preserve">Cancer</t>
@@ -137,22 +137,22 @@
     <t xml:space="preserve">NSC: Healthier Lives</t>
   </si>
   <si>
-    <t xml:space="preserve">0402</t>
+    <t xml:space="preserve">00402</t>
   </si>
   <si>
     <t xml:space="preserve">Cardiovascular disease</t>
   </si>
   <si>
-    <t xml:space="preserve">0403</t>
+    <t xml:space="preserve">00403</t>
   </si>
   <si>
     <t xml:space="preserve">Diabetes</t>
   </si>
   <si>
-    <t xml:space="preserve">0404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0501</t>
+    <t xml:space="preserve">00404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00501</t>
   </si>
   <si>
     <t xml:space="preserve">Metabolic health</t>
@@ -161,25 +161,25 @@
     <t xml:space="preserve">NSC: High Value Nutrition</t>
   </si>
   <si>
-    <t xml:space="preserve">0502</t>
+    <t xml:space="preserve">00502</t>
   </si>
   <si>
     <t xml:space="preserve">Gastrointestinal health</t>
   </si>
   <si>
-    <t xml:space="preserve">0503</t>
+    <t xml:space="preserve">00503</t>
   </si>
   <si>
     <t xml:space="preserve">Immune health</t>
   </si>
   <si>
-    <t xml:space="preserve">0504</t>
+    <t xml:space="preserve">00504</t>
   </si>
   <si>
     <t xml:space="preserve">Weaning foods for health</t>
   </si>
   <si>
-    <t xml:space="preserve">0601</t>
+    <t xml:space="preserve">00601</t>
   </si>
   <si>
     <t xml:space="preserve">Real-time biological heritage assessment</t>
@@ -188,19 +188,19 @@
     <t xml:space="preserve">NSC: New Zealand's Biological Heritage</t>
   </si>
   <si>
-    <t xml:space="preserve">0602</t>
+    <t xml:space="preserve">00602</t>
   </si>
   <si>
     <t xml:space="preserve">Reducing risks and threats across landscapes</t>
   </si>
   <si>
-    <t xml:space="preserve">0603</t>
+    <t xml:space="preserve">00603</t>
   </si>
   <si>
     <t xml:space="preserve">Enhancing and restoring resilient ecosystems</t>
   </si>
   <si>
-    <t xml:space="preserve">0701</t>
+    <t xml:space="preserve">00701</t>
   </si>
   <si>
     <t xml:space="preserve">Greater value in global markets</t>
@@ -209,25 +209,25 @@
     <t xml:space="preserve">NSC: Our Land and Water</t>
   </si>
   <si>
-    <t xml:space="preserve">0702</t>
+    <t xml:space="preserve">00702</t>
   </si>
   <si>
     <t xml:space="preserve">Innovative, resilient land and water use</t>
   </si>
   <si>
-    <t xml:space="preserve">0703</t>
+    <t xml:space="preserve">00703</t>
   </si>
   <si>
     <t xml:space="preserve">Collaborative capacity</t>
   </si>
   <si>
-    <t xml:space="preserve">0704</t>
+    <t xml:space="preserve">00704</t>
   </si>
   <si>
     <t xml:space="preserve">Operating at the nexus</t>
   </si>
   <si>
-    <t xml:space="preserve">0801</t>
+    <t xml:space="preserve">00801</t>
   </si>
   <si>
     <t xml:space="preserve">Rural</t>
@@ -236,61 +236,61 @@
     <t xml:space="preserve">NSC: Resilience to Nature's Challenges</t>
   </si>
   <si>
-    <t xml:space="preserve">0802</t>
+    <t xml:space="preserve">00802</t>
   </si>
   <si>
     <t xml:space="preserve">Urban</t>
   </si>
   <si>
-    <t xml:space="preserve">0803</t>
+    <t xml:space="preserve">00803</t>
   </si>
   <si>
     <t xml:space="preserve">Edge</t>
   </si>
   <si>
-    <t xml:space="preserve">0804</t>
+    <t xml:space="preserve">00804</t>
   </si>
   <si>
     <t xml:space="preserve">Mātauranga Māori</t>
   </si>
   <si>
-    <t xml:space="preserve">0805</t>
+    <t xml:space="preserve">00805</t>
   </si>
   <si>
     <t xml:space="preserve">Governance</t>
   </si>
   <si>
-    <t xml:space="preserve">0806</t>
+    <t xml:space="preserve">00806</t>
   </si>
   <si>
     <t xml:space="preserve">Infrastructure</t>
   </si>
   <si>
-    <t xml:space="preserve">0807</t>
+    <t xml:space="preserve">00807</t>
   </si>
   <si>
     <t xml:space="preserve">Economics</t>
   </si>
   <si>
-    <t xml:space="preserve">0808</t>
+    <t xml:space="preserve">00808</t>
   </si>
   <si>
     <t xml:space="preserve">Culture</t>
   </si>
   <si>
-    <t xml:space="preserve">0809</t>
+    <t xml:space="preserve">00809</t>
   </si>
   <si>
     <t xml:space="preserve">Hazard</t>
   </si>
   <si>
-    <t xml:space="preserve">0810</t>
+    <t xml:space="preserve">00810</t>
   </si>
   <si>
     <t xml:space="preserve">Trajectories</t>
   </si>
   <si>
-    <t xml:space="preserve">0901</t>
+    <t xml:space="preserve">00901</t>
   </si>
   <si>
     <t xml:space="preserve">Vision Mātauranga</t>
@@ -299,25 +299,25 @@
     <t xml:space="preserve">NSC: Science for Technological Innovation</t>
   </si>
   <si>
-    <t xml:space="preserve">0902</t>
+    <t xml:space="preserve">00902</t>
   </si>
   <si>
     <t xml:space="preserve">Materials, Manufacturing and Design</t>
   </si>
   <si>
-    <t xml:space="preserve">0903</t>
+    <t xml:space="preserve">00903</t>
   </si>
   <si>
     <t xml:space="preserve">Sensors, Robotics and Automation</t>
   </si>
   <si>
-    <t xml:space="preserve">0904</t>
+    <t xml:space="preserve">00904</t>
   </si>
   <si>
     <t xml:space="preserve">IT Data Analytics and Modelling</t>
   </si>
   <si>
-    <t xml:space="preserve">1001</t>
+    <t xml:space="preserve">01001</t>
   </si>
   <si>
     <t xml:space="preserve">Our seas</t>
@@ -326,34 +326,34 @@
     <t xml:space="preserve">NSC: Sustainable Seas</t>
   </si>
   <si>
-    <t xml:space="preserve">1002</t>
+    <t xml:space="preserve">01002</t>
   </si>
   <si>
     <t xml:space="preserve">Valuable seas</t>
   </si>
   <si>
-    <t xml:space="preserve">1003</t>
+    <t xml:space="preserve">01003</t>
   </si>
   <si>
     <t xml:space="preserve">Tangaroa</t>
   </si>
   <si>
-    <t xml:space="preserve">1004</t>
+    <t xml:space="preserve">01004</t>
   </si>
   <si>
     <t xml:space="preserve">Dynamic seas</t>
   </si>
   <si>
-    <t xml:space="preserve">1005</t>
+    <t xml:space="preserve">01005</t>
   </si>
   <si>
     <t xml:space="preserve">Managed seas</t>
   </si>
   <si>
-    <t xml:space="preserve">1006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1101</t>
+    <t xml:space="preserve">01006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101</t>
   </si>
   <si>
     <t xml:space="preserve">Engagement</t>
@@ -362,22 +362,22 @@
     <t xml:space="preserve">NSC: The Deep South</t>
   </si>
   <si>
-    <t xml:space="preserve">1102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1103</t>
+    <t xml:space="preserve">01102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01103</t>
   </si>
   <si>
     <t xml:space="preserve">Impacts and implications</t>
   </si>
   <si>
-    <t xml:space="preserve">1104</t>
+    <t xml:space="preserve">01104</t>
   </si>
   <si>
     <t xml:space="preserve">Earth system modelling and prediction</t>
   </si>
   <si>
-    <t xml:space="preserve">1105</t>
+    <t xml:space="preserve">01105</t>
   </si>
   <si>
     <t xml:space="preserve">Processes and observations</t>

</xml_diff>